<commit_message>
adding more array questions
</commit_message>
<xml_diff>
--- a/love_babbar_450/FINAL450.xlsx
+++ b/love_babbar_450/FINAL450.xlsx
@@ -2547,8 +2547,8 @@
   </sheetPr>
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A445" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B106" activeCellId="0" sqref="B106"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A241" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B259" activeCellId="0" sqref="B259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
back after a long time
</commit_message>
<xml_diff>
--- a/love_babbar_450/FINAL450.xlsx
+++ b/love_babbar_450/FINAL450.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="624">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -298,6 +298,9 @@
     <t xml:space="preserve">Smallest Subarray with sum greater than a given value</t>
   </si>
   <si>
+    <t xml:space="preserve">aquire and release strategy</t>
+  </si>
+  <si>
     <t xml:space="preserve">Three way partitioning of an array around a given value</t>
   </si>
   <si>
@@ -319,7 +322,7 @@
     <t xml:space="preserve">Median of 2 sorted arrays of equal size</t>
   </si>
   <si>
-    <t xml:space="preserve">merge two arrays using two pointer i=n-1, j=0|| median=(a1[n-1]+a2[0]) /2</t>
+    <t xml:space="preserve">Hashing -&gt; {a,b,c,d,e,f,g,h....z}  increase index of occuring element</t>
   </si>
   <si>
     <t xml:space="preserve">Median of 2 sorted arrays of different size</t>
@@ -439,9 +442,6 @@
   </si>
   <si>
     <t xml:space="preserve">Find Duplicate characters in a string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hashing -&gt; {a,b,c,d,e,f,g,h....z}  increase index of occuring element</t>
   </si>
   <si>
     <t xml:space="preserve">Why strings are immutable in Java?</t>
@@ -2550,8 +2550,8 @@
   </sheetPr>
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3015,8 +3015,11 @@
       <c r="B36" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>5</v>
+      <c r="C36" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3024,13 +3027,13 @@
         <v>6</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3038,13 +3041,13 @@
         <v>6</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3052,13 +3055,13 @@
         <v>6</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3066,13 +3069,13 @@
         <v>6</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3080,13 +3083,13 @@
         <v>6</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3094,63 +3097,63 @@
         <v>6</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6"/>
       <c r="B43" s="18"/>
       <c r="C43" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6"/>
       <c r="B44" s="18"/>
       <c r="C44" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>5</v>
@@ -3158,24 +3161,24 @@
     </row>
     <row r="48" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>5</v>
@@ -3183,10 +3186,10 @@
     </row>
     <row r="50" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>5</v>
@@ -3194,10 +3197,10 @@
     </row>
     <row r="51" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>5</v>
@@ -3205,24 +3208,24 @@
     </row>
     <row r="52" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>5</v>
@@ -3230,10 +3233,10 @@
     </row>
     <row r="54" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>5</v>
@@ -3246,49 +3249,49 @@
     </row>
     <row r="57" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>104</v>
@@ -3302,7 +3305,7 @@
     </row>
     <row r="61" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>106</v>
@@ -3316,7 +3319,7 @@
     </row>
     <row r="62" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>108</v>
@@ -3330,7 +3333,7 @@
     </row>
     <row r="63" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>110</v>
@@ -3344,7 +3347,7 @@
     </row>
     <row r="64" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>112</v>
@@ -3358,7 +3361,7 @@
     </row>
     <row r="65" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>114</v>
@@ -3372,7 +3375,7 @@
     </row>
     <row r="66" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>116</v>
@@ -3386,7 +3389,7 @@
     </row>
     <row r="67" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>118</v>
@@ -3400,7 +3403,7 @@
     </row>
     <row r="68" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B68" s="20" t="s">
         <v>120</v>
@@ -3411,7 +3414,7 @@
     </row>
     <row r="69" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B69" s="17" t="s">
         <v>121</v>
@@ -3422,7 +3425,7 @@
     </row>
     <row r="70" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>122</v>
@@ -3433,7 +3436,7 @@
     </row>
     <row r="71" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>123</v>
@@ -3447,7 +3450,7 @@
     </row>
     <row r="72" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>125</v>
@@ -3461,7 +3464,7 @@
     </row>
     <row r="73" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>127</v>
@@ -3472,7 +3475,7 @@
     </row>
     <row r="74" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>128</v>
@@ -3483,7 +3486,7 @@
     </row>
     <row r="75" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>129</v>
@@ -3494,7 +3497,7 @@
     </row>
     <row r="76" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>130</v>
@@ -3508,7 +3511,7 @@
     </row>
     <row r="77" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>132</v>
@@ -3519,7 +3522,7 @@
     </row>
     <row r="78" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B78" s="17" t="s">
         <v>133</v>
@@ -3533,7 +3536,7 @@
     </row>
     <row r="79" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>135</v>
@@ -3544,7 +3547,7 @@
     </row>
     <row r="80" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>136</v>
@@ -3555,7 +3558,7 @@
     </row>
     <row r="81" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>137</v>
@@ -3566,7 +3569,7 @@
     </row>
     <row r="82" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>138</v>
@@ -3580,7 +3583,7 @@
     </row>
     <row r="83" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B83" s="7" t="s">
         <v>140</v>
@@ -3594,7 +3597,7 @@
     </row>
     <row r="84" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>142</v>
@@ -3608,7 +3611,7 @@
     </row>
     <row r="85" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B85" s="20" t="s">
         <v>144</v>
@@ -3622,7 +3625,7 @@
     </row>
     <row r="86" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>146</v>
@@ -3633,7 +3636,7 @@
     </row>
     <row r="87" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B87" s="7" t="s">
         <v>147</v>
@@ -3647,7 +3650,7 @@
     </row>
     <row r="88" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>149</v>
@@ -3658,7 +3661,7 @@
     </row>
     <row r="89" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B89" s="17" t="s">
         <v>150</v>
@@ -3669,7 +3672,7 @@
     </row>
     <row r="90" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B90" s="7" t="s">
         <v>151</v>
@@ -3680,7 +3683,7 @@
     </row>
     <row r="91" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>152</v>
@@ -3694,7 +3697,7 @@
     </row>
     <row r="92" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>154</v>
@@ -3708,7 +3711,7 @@
     </row>
     <row r="93" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B93" s="17" t="s">
         <v>156</v>
@@ -3719,7 +3722,7 @@
     </row>
     <row r="94" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>157</v>
@@ -3730,7 +3733,7 @@
     </row>
     <row r="95" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>158</v>
@@ -3741,7 +3744,7 @@
     </row>
     <row r="96" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B96" s="7" t="s">
         <v>159</v>
@@ -3752,7 +3755,7 @@
     </row>
     <row r="97" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B97" s="7" t="s">
         <v>160</v>
@@ -3763,7 +3766,7 @@
     </row>
     <row r="98" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>161</v>
@@ -3774,7 +3777,7 @@
     </row>
     <row r="99" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B99" s="17" t="s">
         <v>162</v>
@@ -3785,7 +3788,7 @@
     </row>
     <row r="100" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B100" s="23" t="s">
         <v>163</v>
@@ -3796,7 +3799,7 @@
     </row>
     <row r="101" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B101" s="24" t="s">
         <v>164</v>
@@ -3807,7 +3810,7 @@
     </row>
     <row r="102" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B102" s="24" t="s">
         <v>165</v>
@@ -3818,7 +3821,7 @@
     </row>
     <row r="103" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B103" s="23" t="s">
         <v>166</v>
@@ -3940,7 +3943,7 @@
         <v>8</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8213,7 +8216,7 @@
       </c>
       <c r="C492" s="35" t="n">
         <f aca="false">COUNTIF(C6:C490,"Yes")</f>
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>